<commit_message>
Proyecto concluido, ya actualiza datos Nota: despues de ingresar un nuevo evento debe actualizarse la pagina para evitar error al querere actualizar ese nuevo registro ingresado
</commit_message>
<xml_diff>
--- a/Relacion Tablas Agenda.xlsx
+++ b/Relacion Tablas Agenda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dbphp\Evaluacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7925F67-888C-47E4-99DD-881396576C9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD81A01-E671-420A-B531-0763A17AC88E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="870" windowWidth="21600" windowHeight="11385" xr2:uid="{3D156311-6F60-4FFD-960B-5C7E2971DD77}"/>
+    <workbookView xWindow="-22605" yWindow="2100" windowWidth="21600" windowHeight="11385" xr2:uid="{3D156311-6F60-4FFD-960B-5C7E2971DD77}"/>
   </bookViews>
   <sheets>
     <sheet name="RELACION TABLAS BANCOS-CONTABIL" sheetId="1" r:id="rId1"/>
@@ -206,15 +206,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1752600</xdr:colOff>
+      <xdr:colOff>1762125</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -229,8 +229,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2524125" y="1371600"/>
-          <a:ext cx="790575" cy="1257300"/>
+          <a:off x="2533650" y="1295400"/>
+          <a:ext cx="809625" cy="1362075"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -579,7 +579,7 @@
   <dimension ref="B2:F20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,21 +698,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FFF190D43C9EF342A9E258A74795CC5C" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="160916fe19e32a8e8bc552a2160b1b62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="68d204b8-073e-41d3-8aeb-97f599785209" xmlns:ns4="ce79a6c9-5888-4498-a25d-12d1ca8e23d5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f113c49ad43d2d642aab4bfcfbf5fbe6" ns3:_="" ns4:_="">
     <xsd:import namespace="68d204b8-073e-41d3-8aeb-97f599785209"/>
@@ -921,32 +906,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3C8CB4E-E9A9-4008-97D8-A7795963F070}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ce79a6c9-5888-4498-a25d-12d1ca8e23d5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="68d204b8-073e-41d3-8aeb-97f599785209"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9731F518-41EB-49EA-AC03-FF9F03DE7CBD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFDE2B8E-20BC-46AF-99E8-E9DEB0733411}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -963,4 +938,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9731F518-41EB-49EA-AC03-FF9F03DE7CBD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3C8CB4E-E9A9-4008-97D8-A7795963F070}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ce79a6c9-5888-4498-a25d-12d1ca8e23d5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="68d204b8-073e-41d3-8aeb-97f599785209"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>